<commit_message>
figure out picture index name problem
</commit_message>
<xml_diff>
--- a/code/Hae.xlsx
+++ b/code/Hae.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\github\Digital_Watermarking-LSB-pair\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\github\Digital_Watermarking-LSB-pair\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B1166A8C-6816-4D3A-AD57-18954EFFB13A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{56F99312-DBF7-4250-A860-74D1F65C7367}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20865" windowHeight="10590" xr2:uid="{C124BF73-661B-4716-ADFD-5926FEDD4A46}"/>
   </bookViews>
@@ -28,18 +28,23 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Image Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LSB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LSB-DES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LSB-pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LSB-pair1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fix missing judgement condition
fix the f^cking bug
</commit_message>
<xml_diff>
--- a/code/Hae.xlsx
+++ b/code/Hae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\github\Digital_Watermarking-LSB-pair\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C8DACF0A-3E02-470C-8D4E-A85C470E9914}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{93346523-FC9B-486C-939B-D30778313FCD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20865" windowHeight="10590" xr2:uid="{805C2402-24A8-48E7-8056-38FCBFFD8019}"/>
   </bookViews>
@@ -505,133 +505,106 @@
         <v>47386</v>
       </c>
       <c r="D2">
-        <v>46390</v>
+        <v>47390</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>10</v>
-      </c>
       <c r="B3">
-        <v>44090</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>44086</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>42300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>100</v>
-      </c>
       <c r="B4">
-        <v>47274</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>47274</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>45976</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>11</v>
-      </c>
       <c r="B5">
-        <v>47064</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>47064</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>44536</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>12</v>
-      </c>
       <c r="B6">
-        <v>44152</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>44152</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>42264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>13</v>
-      </c>
       <c r="B7">
-        <v>41396</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>41392</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>39242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>14</v>
-      </c>
       <c r="B8">
-        <v>25276</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>25292</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>25240</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>15</v>
-      </c>
       <c r="B9">
-        <v>42902</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>42902</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>41938</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>16</v>
-      </c>
       <c r="B10">
-        <v>41808</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>41808</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>40114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>17</v>
-      </c>
       <c r="B11">
-        <v>52194</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>52194</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>51618</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
strat doing dual function
</commit_message>
<xml_diff>
--- a/code/Hae.xlsx
+++ b/code/Hae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\github\Digital_Watermarking-LSB-pair\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{93346523-FC9B-486C-939B-D30778313FCD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{345042DD-4E3D-4159-9CAF-1F2C8A44C8FB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20865" windowHeight="10590" xr2:uid="{805C2402-24A8-48E7-8056-38FCBFFD8019}"/>
   </bookViews>
@@ -509,1092 +509,1389 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10</v>
+      </c>
       <c r="B3">
-        <v>0</v>
+        <v>44090</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>44086</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>44086</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>100</v>
+      </c>
       <c r="B4">
-        <v>0</v>
+        <v>47274</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>47274</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>47274</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>11</v>
+      </c>
       <c r="B5">
-        <v>0</v>
+        <v>47064</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>47064</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>47052</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>12</v>
+      </c>
       <c r="B6">
-        <v>0</v>
+        <v>44152</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>44152</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>44152</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>13</v>
+      </c>
       <c r="B7">
-        <v>0</v>
+        <v>41396</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>41392</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>41392</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>14</v>
+      </c>
       <c r="B8">
-        <v>0</v>
+        <v>25276</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>25292</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>25732</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>15</v>
+      </c>
       <c r="B9">
-        <v>0</v>
+        <v>42902</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>42902</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>42902</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>16</v>
+      </c>
       <c r="B10">
-        <v>0</v>
+        <v>41808</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>41808</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>41808</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>17</v>
+      </c>
       <c r="B11">
-        <v>0</v>
+        <v>52194</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>52194</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>52194</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>18</v>
+      </c>
       <c r="B12">
-        <v>0</v>
+        <v>55006</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>55006</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>55006</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>19</v>
+      </c>
       <c r="B13">
-        <v>0</v>
+        <v>48456</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>48456</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>48456</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
       <c r="B14">
-        <v>0</v>
+        <v>27924</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>27924</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>28096</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>20</v>
+      </c>
       <c r="B15">
-        <v>0</v>
+        <v>21808</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>21628</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>21816</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>21</v>
+      </c>
       <c r="B16">
-        <v>0</v>
+        <v>41820</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>41820</v>
       </c>
       <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41820</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>22</v>
+      </c>
       <c r="B17">
-        <v>0</v>
+        <v>40198</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>40198</v>
       </c>
       <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+        <v>40198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>23</v>
+      </c>
       <c r="B18">
-        <v>0</v>
+        <v>43164</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>43164</v>
       </c>
       <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>24</v>
+      </c>
       <c r="B19">
-        <v>0</v>
+        <v>44764</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>44764</v>
       </c>
       <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+        <v>44760</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>25</v>
+      </c>
       <c r="B20">
-        <v>0</v>
+        <v>45152</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>45148</v>
       </c>
       <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+        <v>45148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>26</v>
+      </c>
       <c r="B21">
-        <v>0</v>
+        <v>43024</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>43024</v>
       </c>
       <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>27</v>
+      </c>
       <c r="B22">
-        <v>0</v>
+        <v>43842</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>43842</v>
       </c>
       <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43842</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>28</v>
+      </c>
       <c r="B23">
-        <v>0</v>
+        <v>45848</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>45848</v>
       </c>
       <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+        <v>45848</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>29</v>
+      </c>
       <c r="B24">
-        <v>0</v>
+        <v>34162</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>34178</v>
       </c>
       <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+        <v>34542</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
       <c r="B25">
-        <v>0</v>
+        <v>42168</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>42168</v>
       </c>
       <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>30</v>
+      </c>
       <c r="B26">
-        <v>0</v>
+        <v>43142</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>43142</v>
       </c>
       <c r="D26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>31</v>
+      </c>
       <c r="B27">
-        <v>0</v>
+        <v>42988</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>42988</v>
       </c>
       <c r="D27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>32</v>
+      </c>
       <c r="B28">
-        <v>0</v>
+        <v>44382</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>44382</v>
       </c>
       <c r="D28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+        <v>44382</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>33</v>
+      </c>
       <c r="B29">
-        <v>0</v>
+        <v>36372</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>36372</v>
       </c>
       <c r="D29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+        <v>36656</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>34</v>
+      </c>
       <c r="B30">
-        <v>0</v>
+        <v>45382</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>45382</v>
       </c>
       <c r="D30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+        <v>45382</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>35</v>
+      </c>
       <c r="B31">
-        <v>0</v>
+        <v>37270</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>37258</v>
       </c>
       <c r="D31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+        <v>37090</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>36</v>
+      </c>
       <c r="B32">
-        <v>0</v>
+        <v>43858</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>43858</v>
       </c>
       <c r="D32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43858</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>37</v>
+      </c>
       <c r="B33">
-        <v>0</v>
+        <v>39150</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>38842</v>
       </c>
       <c r="D33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+        <v>38898</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>38</v>
+      </c>
       <c r="B34">
-        <v>0</v>
+        <v>47016</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>47016</v>
       </c>
       <c r="D34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+        <v>47016</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>39</v>
+      </c>
       <c r="B35">
-        <v>0</v>
+        <v>20342</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>20090</v>
       </c>
       <c r="D35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+        <v>19986</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>4</v>
+      </c>
       <c r="B36">
-        <v>0</v>
+        <v>62634</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>62314</v>
       </c>
       <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+        <v>62098</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>40</v>
+      </c>
       <c r="B37">
-        <v>0</v>
+        <v>54428</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>54428</v>
       </c>
       <c r="D37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+        <v>54428</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>41</v>
+      </c>
       <c r="B38">
-        <v>0</v>
+        <v>49324</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>49316</v>
       </c>
       <c r="D38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+        <v>49316</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>42</v>
+      </c>
       <c r="B39">
-        <v>0</v>
+        <v>44556</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>44556</v>
       </c>
       <c r="D39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+        <v>44560</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>43</v>
+      </c>
       <c r="B40">
-        <v>0</v>
+        <v>47892</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>47572</v>
       </c>
       <c r="D40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+        <v>47932</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>44</v>
+      </c>
       <c r="B41">
-        <v>0</v>
+        <v>55342</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>55342</v>
       </c>
       <c r="D41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+        <v>55342</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>45</v>
+      </c>
       <c r="B42">
-        <v>0</v>
+        <v>64300</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>64296</v>
       </c>
       <c r="D42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+        <v>64296</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>46</v>
+      </c>
       <c r="B43">
-        <v>0</v>
+        <v>61354</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>61350</v>
       </c>
       <c r="D43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+        <v>61342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>47</v>
+      </c>
       <c r="B44">
-        <v>0</v>
+        <v>45138</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>45142</v>
       </c>
       <c r="D44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>48</v>
+      </c>
       <c r="B45">
-        <v>0</v>
+        <v>35544</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>35396</v>
       </c>
       <c r="D45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
+        <v>35172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>49</v>
+      </c>
       <c r="B46">
-        <v>0</v>
+        <v>43624</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>43624</v>
       </c>
       <c r="D46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43624</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>5</v>
+      </c>
       <c r="B47">
-        <v>0</v>
+        <v>43042</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>43042</v>
       </c>
       <c r="D47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>50</v>
+      </c>
       <c r="B48">
-        <v>0</v>
+        <v>43774</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>43774</v>
       </c>
       <c r="D48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43774</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>51</v>
+      </c>
       <c r="B49">
-        <v>0</v>
+        <v>43672</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>43660</v>
       </c>
       <c r="D49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43644</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>52</v>
+      </c>
       <c r="B50">
-        <v>0</v>
+        <v>43894</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>43890</v>
       </c>
       <c r="D50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43878</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>53</v>
+      </c>
       <c r="B51">
-        <v>0</v>
+        <v>41880</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>41880</v>
       </c>
       <c r="D51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41880</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>54</v>
+      </c>
       <c r="B52">
-        <v>0</v>
+        <v>43202</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>43198</v>
       </c>
       <c r="D52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43182</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>55</v>
+      </c>
       <c r="B53">
-        <v>0</v>
+        <v>41430</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>41430</v>
       </c>
       <c r="D53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41430</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>56</v>
+      </c>
       <c r="B54">
-        <v>0</v>
+        <v>44344</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>44344</v>
       </c>
       <c r="D54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+        <v>44344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>57</v>
+      </c>
       <c r="B55">
-        <v>0</v>
+        <v>39580</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>39580</v>
       </c>
       <c r="D55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+        <v>39580</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>58</v>
+      </c>
       <c r="B56">
-        <v>0</v>
+        <v>42370</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>42370</v>
       </c>
       <c r="D56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42370</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>59</v>
+      </c>
       <c r="B57">
-        <v>0</v>
+        <v>43820</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>43820</v>
       </c>
       <c r="D57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43820</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>6</v>
+      </c>
       <c r="B58">
-        <v>0</v>
+        <v>43442</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>43442</v>
       </c>
       <c r="D58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43442</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>60</v>
+      </c>
       <c r="B59">
-        <v>0</v>
+        <v>42996</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>42996</v>
       </c>
       <c r="D59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>61</v>
+      </c>
       <c r="B60">
-        <v>0</v>
+        <v>32206</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>32206</v>
       </c>
       <c r="D60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+        <v>32206</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>62</v>
+      </c>
       <c r="B61">
-        <v>0</v>
+        <v>31696</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>31696</v>
       </c>
       <c r="D61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+        <v>31696</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>63</v>
+      </c>
       <c r="B62">
-        <v>0</v>
+        <v>37988</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>37820</v>
       </c>
       <c r="D62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+        <v>37860</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>64</v>
+      </c>
       <c r="B63">
-        <v>0</v>
+        <v>31936</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>31952</v>
       </c>
       <c r="D63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+        <v>32266</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>65</v>
+      </c>
       <c r="B64">
-        <v>0</v>
+        <v>28060</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>28060</v>
       </c>
       <c r="D64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+        <v>28810</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>66</v>
+      </c>
       <c r="B65">
-        <v>0</v>
+        <v>36198</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>36198</v>
       </c>
       <c r="D65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+        <v>36198</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>67</v>
+      </c>
       <c r="B66">
-        <v>0</v>
+        <v>45478</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>45482</v>
       </c>
       <c r="D66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+        <v>45486</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>68</v>
+      </c>
       <c r="B67">
-        <v>0</v>
+        <v>39432</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>39432</v>
       </c>
       <c r="D67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+        <v>39634</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>69</v>
+      </c>
       <c r="B68">
-        <v>0</v>
+        <v>39754</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>39754</v>
       </c>
       <c r="D68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+        <v>39754</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>7</v>
+      </c>
       <c r="B69">
-        <v>0</v>
+        <v>37430</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>37430</v>
       </c>
       <c r="D69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+        <v>37430</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>70</v>
+      </c>
       <c r="B70">
-        <v>0</v>
+        <v>41268</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>41268</v>
       </c>
       <c r="D70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41268</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>71</v>
+      </c>
       <c r="B71">
-        <v>0</v>
+        <v>42628</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>42628</v>
       </c>
       <c r="D71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42628</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>72</v>
+      </c>
       <c r="B72">
-        <v>0</v>
+        <v>42274</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>42274</v>
       </c>
       <c r="D72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42274</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>73</v>
+      </c>
       <c r="B73">
-        <v>0</v>
+        <v>43046</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>43046</v>
       </c>
       <c r="D73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>74</v>
+      </c>
       <c r="B74">
-        <v>0</v>
+        <v>43824</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>43824</v>
       </c>
       <c r="D74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43824</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>75</v>
+      </c>
       <c r="B75">
-        <v>0</v>
+        <v>42556</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>42556</v>
       </c>
       <c r="D75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42556</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>76</v>
+      </c>
       <c r="B76">
-        <v>0</v>
+        <v>43350</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>43194</v>
       </c>
       <c r="D76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43212</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>77</v>
+      </c>
       <c r="B77">
-        <v>0</v>
+        <v>43068</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>43040</v>
       </c>
       <c r="D77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>78</v>
+      </c>
       <c r="B78">
-        <v>0</v>
+        <v>43360</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>43360</v>
       </c>
       <c r="D78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43360</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>79</v>
+      </c>
       <c r="B79">
-        <v>0</v>
+        <v>41874</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>41874</v>
       </c>
       <c r="D79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41874</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>8</v>
+      </c>
       <c r="B80">
-        <v>0</v>
+        <v>46190</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>46190</v>
       </c>
       <c r="D80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+        <v>46190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
       <c r="B81">
-        <v>0</v>
+        <v>41366</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>41366</v>
       </c>
       <c r="D81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41366</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
       <c r="B82">
-        <v>0</v>
+        <v>45320</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>45320</v>
       </c>
       <c r="D82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+        <v>45320</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
       <c r="B83">
-        <v>0</v>
+        <v>49088</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>49088</v>
       </c>
       <c r="D83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+        <v>49092</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
       <c r="B84">
-        <v>0</v>
+        <v>33506</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>33506</v>
       </c>
       <c r="D84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+        <v>33972</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
       <c r="B85">
-        <v>0</v>
+        <v>30120</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>30120</v>
       </c>
       <c r="D85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+        <v>30120</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
       <c r="B86">
-        <v>0</v>
+        <v>41180</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>41180</v>
       </c>
       <c r="D86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41180</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
       <c r="B87">
-        <v>0</v>
+        <v>30796</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>30796</v>
       </c>
       <c r="D87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+        <v>31308</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
       <c r="B88">
-        <v>0</v>
+        <v>41810</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>41810</v>
       </c>
       <c r="D88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41810</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
       <c r="B89">
-        <v>0</v>
+        <v>36110</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>36110</v>
       </c>
       <c r="D89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
+        <v>36110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
       <c r="B90">
-        <v>0</v>
+        <v>35966</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>35962</v>
       </c>
       <c r="D90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
+        <v>35962</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>9</v>
+      </c>
       <c r="B91">
-        <v>0</v>
+        <v>40528</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>40528</v>
       </c>
       <c r="D91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
+        <v>40528</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>90</v>
+      </c>
       <c r="B92">
-        <v>0</v>
+        <v>44244</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>44244</v>
       </c>
       <c r="D92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
+        <v>44244</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>91</v>
+      </c>
       <c r="B93">
-        <v>0</v>
+        <v>42870</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>42870</v>
       </c>
       <c r="D93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42870</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>92</v>
+      </c>
       <c r="B94">
-        <v>0</v>
+        <v>41420</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>41420</v>
       </c>
       <c r="D94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.2">
+        <v>41420</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>93</v>
+      </c>
       <c r="B95">
-        <v>0</v>
+        <v>45596</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>45596</v>
       </c>
       <c r="D95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.2">
+        <v>45596</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>94</v>
+      </c>
       <c r="B96">
-        <v>0</v>
+        <v>50130</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>50130</v>
       </c>
       <c r="D96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.2">
+        <v>50132</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>95</v>
+      </c>
       <c r="B97">
-        <v>0</v>
+        <v>44170</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>44170</v>
       </c>
       <c r="D97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.2">
+        <v>44170</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>96</v>
+      </c>
       <c r="B98">
-        <v>0</v>
+        <v>48270</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>48270</v>
       </c>
       <c r="D98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.2">
+        <v>48270</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>97</v>
+      </c>
       <c r="B99">
-        <v>0</v>
+        <v>48820</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>48820</v>
       </c>
       <c r="D99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.2">
+        <v>48820</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>98</v>
+      </c>
       <c r="B100">
-        <v>0</v>
+        <v>43588</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>43588</v>
       </c>
       <c r="D100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.2">
+        <v>43588</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>99</v>
+      </c>
       <c r="B101">
-        <v>0</v>
+        <v>46194</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>46194</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>46194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>